<commit_message>
Final Test for the Night, Tableau checked and is working with no real data.
</commit_message>
<xml_diff>
--- a/InvestingData.xlsx
+++ b/InvestingData.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="336">
   <si>
     <t>aapl</t>
   </si>
@@ -742,6 +742,294 @@
   </si>
   <si>
     <t>2021-01-11 01:25:54.312</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:27.922</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.031</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.056</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.079</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.1</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.12</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.141</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.161</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.183</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.201</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.222</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.242</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.265</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.283</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.304</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.322</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.339</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.356</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.372</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.388</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.408</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.424</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.445</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.463</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.478</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.492</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.506</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.52</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.535</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.549</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.562</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.578</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.592</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.607</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.623</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.639</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.653</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.666</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.678</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.7</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.713</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.724</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.735</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.75</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.759</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.769</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.783</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.795</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.808</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.82</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.832</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.844</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.856</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.87</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.883</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.894</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.905</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.917</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.928</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.937</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.947</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.958</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.969</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.981</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:28.995</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:29.007</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:29.018</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:29.029</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:29.041</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:29.052</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:29.064</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:29.074</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:29.085</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:29.097</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:29.106</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:29.115</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:29.125</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:29.135</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:29.147</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:29.16</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:29.172</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:29.186</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:29.198</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:29.214</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:29.224</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:29.236</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:29.246</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:29.26</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:29.27</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:29.28</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:29.289</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:29.299</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:29.308</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:29.316</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:29.327</t>
+  </si>
+  <si>
+    <t>2021-01-11 01:33:29.337</t>
   </si>
 </sst>
 </file>
@@ -2555,7 +2843,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{541144C4-A731-4EED-9617-9A606B501EA9}">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B134"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
@@ -2867,6 +3155,774 @@
         <v>239</v>
       </c>
     </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>2</v>
+      </c>
+      <c r="B40" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>3</v>
+      </c>
+      <c r="B41" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>4</v>
+      </c>
+      <c r="B42" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>6</v>
+      </c>
+      <c r="B44" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>0</v>
+      </c>
+      <c r="B45" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>7</v>
+      </c>
+      <c r="B46" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>8</v>
+      </c>
+      <c r="B47" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>9</v>
+      </c>
+      <c r="B48" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>10</v>
+      </c>
+      <c r="B49" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>11</v>
+      </c>
+      <c r="B50" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>12</v>
+      </c>
+      <c r="B51" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>13</v>
+      </c>
+      <c r="B52" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>14</v>
+      </c>
+      <c r="B53" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>15</v>
+      </c>
+      <c r="B54" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>16</v>
+      </c>
+      <c r="B55" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>17</v>
+      </c>
+      <c r="B56" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>18</v>
+      </c>
+      <c r="B57" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>19</v>
+      </c>
+      <c r="B58" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>20</v>
+      </c>
+      <c r="B59" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>21</v>
+      </c>
+      <c r="B60" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>22</v>
+      </c>
+      <c r="B61" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>23</v>
+      </c>
+      <c r="B62" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>24</v>
+      </c>
+      <c r="B63" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s">
+        <v>25</v>
+      </c>
+      <c r="B64" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s">
+        <v>26</v>
+      </c>
+      <c r="B65" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s">
+        <v>27</v>
+      </c>
+      <c r="B66" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s">
+        <v>28</v>
+      </c>
+      <c r="B67" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s">
+        <v>29</v>
+      </c>
+      <c r="B68" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s">
+        <v>30</v>
+      </c>
+      <c r="B69" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s">
+        <v>31</v>
+      </c>
+      <c r="B70" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s">
+        <v>32</v>
+      </c>
+      <c r="B71" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s">
+        <v>33</v>
+      </c>
+      <c r="B72" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s">
+        <v>34</v>
+      </c>
+      <c r="B73" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s">
+        <v>35</v>
+      </c>
+      <c r="B74" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s">
+        <v>36</v>
+      </c>
+      <c r="B75" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s">
+        <v>37</v>
+      </c>
+      <c r="B76" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s">
+        <v>38</v>
+      </c>
+      <c r="B77" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s">
+        <v>39</v>
+      </c>
+      <c r="B78" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s">
+        <v>40</v>
+      </c>
+      <c r="B79" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s">
+        <v>41</v>
+      </c>
+      <c r="B80" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s">
+        <v>42</v>
+      </c>
+      <c r="B81" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s">
+        <v>43</v>
+      </c>
+      <c r="B82" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s">
+        <v>44</v>
+      </c>
+      <c r="B83" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s">
+        <v>45</v>
+      </c>
+      <c r="B84" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s">
+        <v>46</v>
+      </c>
+      <c r="B85" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s">
+        <v>47</v>
+      </c>
+      <c r="B86" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="s">
+        <v>48</v>
+      </c>
+      <c r="B87" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="s">
+        <v>49</v>
+      </c>
+      <c r="B88" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="s">
+        <v>50</v>
+      </c>
+      <c r="B89" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="s">
+        <v>51</v>
+      </c>
+      <c r="B90" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="s">
+        <v>52</v>
+      </c>
+      <c r="B91" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="s">
+        <v>53</v>
+      </c>
+      <c r="B92" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="s">
+        <v>54</v>
+      </c>
+      <c r="B93" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="s">
+        <v>55</v>
+      </c>
+      <c r="B94" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="s">
+        <v>56</v>
+      </c>
+      <c r="B95" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="s">
+        <v>57</v>
+      </c>
+      <c r="B96" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="s">
+        <v>58</v>
+      </c>
+      <c r="B97" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="s">
+        <v>59</v>
+      </c>
+      <c r="B98" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="s">
+        <v>60</v>
+      </c>
+      <c r="B99" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="s">
+        <v>61</v>
+      </c>
+      <c r="B100" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="s">
+        <v>62</v>
+      </c>
+      <c r="B101" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="s">
+        <v>63</v>
+      </c>
+      <c r="B102" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="s">
+        <v>64</v>
+      </c>
+      <c r="B103" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="s">
+        <v>65</v>
+      </c>
+      <c r="B104" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="s">
+        <v>66</v>
+      </c>
+      <c r="B105" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="s">
+        <v>67</v>
+      </c>
+      <c r="B106" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="s">
+        <v>68</v>
+      </c>
+      <c r="B107" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="s">
+        <v>69</v>
+      </c>
+      <c r="B108" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="s">
+        <v>70</v>
+      </c>
+      <c r="B109" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="s">
+        <v>71</v>
+      </c>
+      <c r="B110" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="s">
+        <v>72</v>
+      </c>
+      <c r="B111" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="s">
+        <v>73</v>
+      </c>
+      <c r="B112" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="s">
+        <v>74</v>
+      </c>
+      <c r="B113" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="s">
+        <v>75</v>
+      </c>
+      <c r="B114" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="s">
+        <v>76</v>
+      </c>
+      <c r="B115" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="s">
+        <v>77</v>
+      </c>
+      <c r="B116" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="s">
+        <v>78</v>
+      </c>
+      <c r="B117" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="s">
+        <v>79</v>
+      </c>
+      <c r="B118" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="s">
+        <v>80</v>
+      </c>
+      <c r="B119" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="s">
+        <v>81</v>
+      </c>
+      <c r="B120" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="s">
+        <v>82</v>
+      </c>
+      <c r="B121" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="s">
+        <v>83</v>
+      </c>
+      <c r="B122" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="s">
+        <v>84</v>
+      </c>
+      <c r="B123" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="s">
+        <v>85</v>
+      </c>
+      <c r="B124" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="s">
+        <v>86</v>
+      </c>
+      <c r="B125" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="s">
+        <v>87</v>
+      </c>
+      <c r="B126" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="s">
+        <v>88</v>
+      </c>
+      <c r="B127" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="s">
+        <v>89</v>
+      </c>
+      <c r="B128" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="s">
+        <v>90</v>
+      </c>
+      <c r="B129" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="s">
+        <v>91</v>
+      </c>
+      <c r="B130" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="s">
+        <v>92</v>
+      </c>
+      <c r="B131" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="s">
+        <v>93</v>
+      </c>
+      <c r="B132" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="s">
+        <v>94</v>
+      </c>
+      <c r="B133" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="s">
+        <v>95</v>
+      </c>
+      <c r="B134" t="s">
+        <v>335</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>